<commit_message>
[upd] manually corrected Udofot's stress patterns
</commit_message>
<xml_diff>
--- a/data/external/pilot_comparison/pilot_comparison_w_udofot.xlsx
+++ b/data/external/pilot_comparison/pilot_comparison_w_udofot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryuki/Development/l2speech-ree-group-proj/data/external/pilot_comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06AB359E-6E1F-584A-8F36-6291A8C05554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4558F2-A393-8D46-8257-7AEC12CC0F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16020" xr2:uid="{6387D3C8-8653-394B-B616-04AF64C5039D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="28">
   <si>
     <t>to</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>Control</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>W</t>
@@ -511,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC1B69A-26C6-3B4B-9248-1AB0ABDDAE09}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -523,16 +520,16 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -566,55 +563,53 @@
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>11</v>
@@ -623,299 +618,299 @@
         <v>11</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>11</v>
@@ -924,40 +919,40 @@
     <row r="11" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>